<commit_message>
US5 Updated Test Case
The test cases are corrected and updated in this version.
</commit_message>
<xml_diff>
--- a/SimpCity US5Test Cases.xlsx
+++ b/SimpCity US5Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86355B44-DC00-49E2-8B0F-77D95DD2E5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D337042F-27BA-40A2-B223-C3760CC0DA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t>Test Scenarios for SimpCity</t>
   </si>
@@ -151,13 +151,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>The number "0" is inputted by the user</t>
-  </si>
-  <si>
-    <t>Before: Start New Game option is selected
-After:  Your Choice? 0</t>
-  </si>
-  <si>
     <t>Equivalence</t>
   </si>
   <si>
@@ -165,9 +158,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>The number "0" to "5" is not inputted by the user</t>
   </si>
   <si>
     <t>Before:</t>
@@ -205,109 +195,62 @@
 After: Your Choice? 2</t>
   </si>
   <si>
-    <t>The number "3" is inputted by the user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The user enters an option value of the numeric interger "3" when the message "Your Choice?" prompted </t>
-  </si>
-  <si>
-    <t>Before: Start New Game option is selected
-After:  Your Choice? 3</t>
-  </si>
-  <si>
-    <t>Remanining buildings available for the users to select is displayed to the users.</t>
-  </si>
-  <si>
-    <t>The number "4" is inputted by the user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The user enters an option value of the numeric interger "4" when the message "Your Choice?" prompted </t>
-  </si>
-  <si>
-    <t>Before: Start New Game option is selected
-After:  Your Choice? 4</t>
-  </si>
-  <si>
-    <t>The computation of score accmulated for each building and the current "Total Score: " is displayed to the users</t>
-  </si>
-  <si>
-    <t>The number "5" is inputted by the user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The user enters an option value of the numeric interger "5" when the message "Your Choice?" prompted </t>
-  </si>
-  <si>
-    <t>Before: Start New Game option is selected
-After:  Your Choice? 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A verification message "Game saved" is displayed to indicate that the game was saved sucessfully </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The user enters an option value of the numeric interger "0" when the message "Your Choice?" is prompted </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user return to the main menu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The user enters an option value that is not a numeric interger of  "0" to "5" when prompted </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Before: Start New Game option is selected
-After: [Any value expect "0" to "5"" </t>
-  </si>
-  <si>
-    <t>An error message will be displayed to remind the users only number "0" to  "5" will be accepted and the message "Build where?" will not be prompted.</t>
-  </si>
-  <si>
     <t>The number from "0" to "5" is not inputted by the user, then the user try again with the number "2", then with value from "3" to "5" or "0"</t>
   </si>
   <si>
-    <t xml:space="preserve">1. The user enters an option value that is not a numeric interger of  "0" to "5" when prompted 
+    <t>After:
+1. Value from "3" to "5" or "0".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The system shall process each option value from the menu as accordance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary </t>
+  </si>
+  <si>
+    <t>After:
+2. Nominal value: 2</t>
+  </si>
+  <si>
+    <t>2. The message "Build where?" shall be displayed to prompt the users to enter the location of the selected building to be placed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After:
+3. [Any value expect "0" to "5"" </t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. The user enters an option value that is not a numeric interger of  "0" to "2" when prompted 
 2. The user enters "0" to exit to the main menu
 3. The user enters an option value of the numeric interger "2" when the message "Your Choice?" is prompted 
-4.2. The user enters "0" to exit to the main menu
-5. The users enter an option value of the numeric integer from "3" to "5" or "0" </t>
-  </si>
-  <si>
-    <t>test failing is like for error message like you expect it to appear, out of bound, go the right position</t>
+4.The user enters "0" to exit to the main menu
+5. The user enters any value from "3" to "5"
+6. The user enters "0" to exit to the main menu
+7. The users enter an option value that is not from "0" to "5" and is not a numeric interger"
+</t>
+  </si>
+  <si>
+    <t>3. The system shall not return any prompt or input.</t>
+  </si>
+  <si>
+    <t>4. The system shall display an error message shall be displayed to remind the users only number "0" to "5" will be accepted.</t>
   </si>
   <si>
     <t>After:
-1. Value from "3" to "5" or "0".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. The system shall process each option value from the menu as accordance. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boundary </t>
-  </si>
-  <si>
-    <t>After:
-2. Nominal value: 2</t>
-  </si>
-  <si>
-    <t>2. The message "Build where?" shall be displayed to prompt the users to enter the location of the selected building to be placed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After:
-3. [Any value expect "0" to "5"" </t>
-  </si>
-  <si>
-    <t>3. The system shall display an error message shall be displayed to remind the users only number "0" to "5" will be accepted.</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Pending</t>
+4. [Any value expect "0" to "5" and not a numeric interger}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +318,12 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -730,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -798,9 +747,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -946,9 +892,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -964,26 +934,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,58 +967,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>685800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CDB1B18-E62B-4320-BB46-439131C4AB87}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{02FB2E92-4919-40D2-995E-B06DBEB5C7F9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14525625" y="10267950"/>
-          <a:ext cx="4562475" cy="2552700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1351,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,696 +1286,619 @@
     <col min="11" max="11" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="87" t="s">
+    <row r="1" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27"/>
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="62"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="61"/>
       <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
-      <c r="B2" s="81" t="s">
+    <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50"/>
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="83"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="88"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="88" t="s">
+      <c r="F2" s="83"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="81" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="82"/>
-    </row>
-    <row r="3" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="38" t="s">
+      <c r="K2" s="89"/>
+    </row>
+    <row r="3" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="59" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="59" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="47" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="63" t="s">
+    <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="58" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="58" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="56" t="s">
+      <c r="I4" s="59"/>
+      <c r="J4" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="47" t="s">
+      <c r="K4" s="46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="43" t="s">
+    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45"/>
+      <c r="B5" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="70">
         <v>44545</v>
       </c>
       <c r="D5" s="19"/>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="72" t="s">
+      <c r="F5" s="69"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="69"/>
-      <c r="J5" s="56" t="s">
+      <c r="I5" s="68"/>
+      <c r="J5" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="47" t="s">
+      <c r="K5" s="46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="77" t="s">
-        <v>84</v>
+      <c r="C6" s="76" t="s">
+        <v>61</v>
       </c>
       <c r="D6" s="19"/>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="77" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="68" t="s">
+      <c r="F6" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="78" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="43" t="s">
+      <c r="I6" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="83" t="s">
+    <row r="7" spans="1:21" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="83"/>
+      <c r="C7" s="90"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="83"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="83" t="s">
+      <c r="F7" s="90"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="83"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="66"/>
-      <c r="B8" s="73" t="s">
+      <c r="I7" s="90"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="65"/>
+      <c r="B8" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="22"/>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="75" t="s">
+      <c r="G8" s="41"/>
+      <c r="H8" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="64" t="s">
+      <c r="J8" s="48"/>
+      <c r="K8" s="49"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="80"/>
+      <c r="D9" s="79"/>
       <c r="E9" s="1"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="65" t="s">
+      <c r="G9" s="35"/>
+      <c r="H9" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="19"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
       <c r="D10" s="9"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="68" t="s">
+      <c r="F10" s="32"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="36"/>
+      <c r="J10" s="35"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="I12" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="34" t="s">
         <v>38</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+    <row r="13" spans="1:21" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="80">
         <v>1</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="F13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="1:21" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="80">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="C14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="E14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="I14" s="22"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="22"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="91">
+        <v>3</v>
+      </c>
+      <c r="B15" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="E15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="22"/>
-    </row>
-    <row r="14" spans="1:11" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
-        <v>2</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="G15" s="84" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="22"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="92"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E16" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="31" t="s">
+      <c r="F16" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="84"/>
+      <c r="H16" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="22"/>
-    </row>
-    <row r="15" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
-        <v>3</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="92"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E17" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="F17" s="87"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="22"/>
+    </row>
+    <row r="18" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="92"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="E18" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="87"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="22"/>
-    </row>
-    <row r="16" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
-        <v>4</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="22"/>
-    </row>
-    <row r="17" spans="1:21" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
-        <v>5</v>
-      </c>
-      <c r="B17" s="17" t="s">
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="93"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="1:21" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="17">
-        <v>6</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="22"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="1:21" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17">
-        <v>7</v>
-      </c>
-      <c r="B19" s="17" t="s">
+      <c r="F19" s="88"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="22"/>
     </row>
-    <row r="20" spans="1:21" ht="184.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="84">
-        <v>8</v>
-      </c>
-      <c r="B20" s="89" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="90" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="22"/>
-      <c r="U20" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="85"/>
-      <c r="B21" s="89"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="91" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="89"/>
-      <c r="H21" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="1:21" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="85"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="92"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="1:21" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="93"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="10"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="10"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="11"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2129,56 +1967,16 @@
       <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="6"/>
+      <c r="B39" s="4"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="6"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="6"/>
+      <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="6"/>
+      <c r="B42" s="4"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
@@ -2201,43 +1999,31 @@
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="4"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="4"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="F16:F19"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H23 I19:I23 J13:J23" xr:uid="{00CE29C5-517E-40B9-9503-E65801202668}">
-      <formula1>"Pass, Fail"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 F6 I6" xr:uid="{7EC201AA-325A-48A0-9DE1-F4D30C6CD250}">
       <formula1>"Pending, In Progress, Done"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H14 J13:J14 H15:J19" xr:uid="{00CE29C5-517E-40B9-9503-E65801202668}">
+      <formula1>"Pass, Fail"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
US5 Test Case Approved
Scrum Master signature for TDA, approved US5
</commit_message>
<xml_diff>
--- a/SimpCity US5Test Cases.xlsx
+++ b/SimpCity US5Test Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem3.2-DevOps\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BB6D92-4873-4BD6-B51E-641B805DD22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D9BD58-895B-4D2E-BC06-3516BA3BA698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US5" sheetId="1" r:id="rId1"/>
@@ -886,52 +886,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,10 +1773,10 @@
   <sheetData>
     <row r="1" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23"/>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
+      <c r="C1" s="92"/>
       <c r="D1" s="49"/>
       <c r="E1" s="46"/>
       <c r="F1" s="51"/>
@@ -1788,24 +1788,24 @@
     </row>
     <row r="2" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="45"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="94"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="88"/>
+      <c r="F2" s="94"/>
       <c r="G2" s="40"/>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="81" t="s">
+      <c r="I2" s="94"/>
+      <c r="J2" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="82"/>
+      <c r="K2" s="95"/>
     </row>
     <row r="3" spans="1:21" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
@@ -1921,20 +1921,20 @@
     </row>
     <row r="7" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="83"/>
+      <c r="C7" s="96"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="83"/>
+      <c r="F7" s="96"/>
       <c r="G7" s="30"/>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="83"/>
+      <c r="I7" s="96"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="60"/>
@@ -1949,7 +1949,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="67" t="s">
@@ -1970,7 +1970,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="71" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="G9" s="30"/>
       <c r="H9" s="59" t="s">
@@ -2114,13 +2114,13 @@
       <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:21" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="84">
+      <c r="A15" s="81">
         <v>3</v>
       </c>
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="85" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -2129,7 +2129,7 @@
       <c r="E15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="89" t="s">
+      <c r="G15" s="88" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="26"/>
@@ -2139,19 +2139,19 @@
       <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:21" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="92"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="94" t="s">
+      <c r="F16" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="89"/>
+      <c r="G16" s="88"/>
       <c r="H16" s="26" t="s">
         <v>41</v>
       </c>
@@ -2164,17 +2164,17 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="351" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="92"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="86"/>
       <c r="D17" s="22" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="95"/>
-      <c r="G17" s="89"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="88"/>
       <c r="H17" s="26" t="s">
         <v>41</v>
       </c>
@@ -2185,17 +2185,17 @@
       <c r="K17" s="18"/>
     </row>
     <row r="18" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="85"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="92"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="95"/>
-      <c r="G18" s="89"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="88"/>
       <c r="H18" s="73" t="s">
         <v>41</v>
       </c>
@@ -2208,17 +2208,17 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="406.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="93"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="76" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="96"/>
-      <c r="G19" s="89"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="26" t="s">
         <v>44</v>
       </c>
@@ -2385,13 +2385,13 @@
       <c r="K26" s="18"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="84">
+      <c r="A27" s="81">
         <v>3</v>
       </c>
-      <c r="B27" s="90" t="s">
+      <c r="B27" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="91" t="s">
+      <c r="C27" s="85" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="20" t="s">
@@ -2400,7 +2400,7 @@
       <c r="E27" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="89" t="s">
+      <c r="G27" s="88" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="79"/>
@@ -2409,19 +2409,19 @@
       <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:11" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="92"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="86"/>
       <c r="D28" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="94" t="s">
+      <c r="F28" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="89"/>
+      <c r="G28" s="88"/>
       <c r="H28" s="79" t="s">
         <v>41</v>
       </c>
@@ -2434,17 +2434,17 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="330.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="85"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="92"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="86"/>
       <c r="D29" s="22" t="s">
         <v>57</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="95"/>
-      <c r="G29" s="89"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="88"/>
       <c r="H29" s="79" t="s">
         <v>41</v>
       </c>
@@ -2455,17 +2455,17 @@
       <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:11" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
-      <c r="B30" s="90"/>
-      <c r="C30" s="92"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="95"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="88"/>
       <c r="H30" s="79" t="s">
         <v>41</v>
       </c>
@@ -2478,17 +2478,17 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="365.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="76" t="s">
         <v>63</v>
       </c>
       <c r="E31" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="96"/>
-      <c r="G31" s="89"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="88"/>
       <c r="H31" s="79" t="s">
         <v>44</v>
       </c>
@@ -2626,11 +2626,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
@@ -2639,11 +2639,11 @@
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="F16:F19"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="F28:F31"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 F6 I6" xr:uid="{7EC201AA-325A-48A0-9DE1-F4D30C6CD250}">

</xml_diff>